<commit_message>
생치 column chart 추가
</commit_message>
<xml_diff>
--- a/hospital.xlsx
+++ b/hospital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngjunna/Github/corona-sickbed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngjunna/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ECD0FE-BCBD-CE4C-AF7F-ACCDCAAE6E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73E724C-37C2-F245-9361-D144BAE5742B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{4E7B2BDB-084F-E141-A5C9-24E5D944D897}"/>
+    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{4E7B2BDB-084F-E141-A5C9-24E5D944D897}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>lat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>동탄성심</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성빈센트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현대병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세종병원</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72E2835-0F31-6D45-9411-3403538554CF}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -667,6 +679,39 @@
         <v>127.080099</v>
       </c>
     </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>37.278156000000003</v>
+      </c>
+      <c r="C18">
+        <v>127.02781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>37.715788000000003</v>
+      </c>
+      <c r="C19">
+        <v>127.179631</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>37.481034000000001</v>
+      </c>
+      <c r="C20">
+        <v>126.79118800000001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>